<commit_message>
GA_00003 and GS_00003 deployment information
- added new instruments to sensor_bulk_load
- updated calibration coefficients for some deployed ADCPs
- GA and GS mooring deployment sheets: updated information for
deployment 3, and added CUID_Recover
</commit_message>
<xml_diff>
--- a/ARCHIVE/deployment/Omaha_Cal_Info_GA02HYPM_00003.xlsx
+++ b/ARCHIVE/deployment/Omaha_Cal_Info_GA02HYPM_00003.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
-  <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="27907"/>
+  <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lgarzio\Desktop\cal sheets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lgarzio/Documents/repo/lgarzio/ooi-integration-fork/asset-management/ARCHIVE/deployment/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24576" windowHeight="9696"/>
+    <workbookView xWindow="38400" yWindow="460" windowWidth="38400" windowHeight="21140" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Moorings" sheetId="2" r:id="rId1"/>
@@ -22,8 +22,11 @@
     <definedName name="_FilterDatabase_0">[1]Moorings!#REF!</definedName>
     <definedName name="_FilterDatabase_0_0_0">[1]Moorings!#REF!</definedName>
   </definedNames>
-  <calcPr calcId="152511" concurrentCalc="0"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -32,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="360" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="359" uniqueCount="94">
   <si>
     <t>Ref Des</t>
   </si>
@@ -176,9 +179,6 @@
   </si>
   <si>
     <t>GA02HYPM-MPM01-02-ZPLSGA010</t>
-  </si>
-  <si>
-    <t>14880</t>
   </si>
   <si>
     <t>Not Deployed</t>
@@ -1409,9 +1409,6 @@
     <xf numFmtId="11" fontId="48" fillId="36" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="44" fillId="37" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="166" fontId="44" fillId="37" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -1421,6 +1418,9 @@
     </xf>
     <xf numFmtId="0" fontId="14" fillId="37" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="14" fillId="0" borderId="3" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="231">
@@ -1732,9 +1732,9 @@
         <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="Yu Gothic Light"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="DengXian Light"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Times New Roman"/>
         <a:font script="Hebr" typeface="Times New Roman"/>
@@ -1767,9 +1767,9 @@
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="Yu Gothic"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="DengXian"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Arial"/>
         <a:font script="Hebr" typeface="Arial"/>
@@ -1975,32 +1975,32 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N16"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="13.5546875" style="3" customWidth="1"/>
+    <col min="1" max="1" width="13.5" style="3" customWidth="1"/>
     <col min="2" max="2" width="16.33203125" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.44140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.44140625" style="15" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.5" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.5" style="15" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.33203125" style="12" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11.33203125" style="9" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="14.33203125" style="12" customWidth="1"/>
-    <col min="8" max="8" width="13.109375" style="3" customWidth="1"/>
-    <col min="9" max="9" width="13.44140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.1640625" style="3" customWidth="1"/>
+    <col min="9" max="9" width="13.5" style="3" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="13.6640625" style="3" customWidth="1"/>
-    <col min="11" max="11" width="11.44140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.5" style="3" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="22.6640625" style="3" customWidth="1"/>
-    <col min="13" max="13" width="17.109375" style="3" customWidth="1"/>
-    <col min="14" max="14" width="17.88671875" style="3" customWidth="1"/>
-    <col min="15" max="16384" width="8.88671875" style="3"/>
+    <col min="13" max="13" width="17.1640625" style="3" customWidth="1"/>
+    <col min="14" max="14" width="17.83203125" style="3" customWidth="1"/>
+    <col min="15" max="16384" width="8.83203125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="7" customFormat="1" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" s="7" customFormat="1" ht="28" x14ac:dyDescent="0.2">
       <c r="A1" s="33" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>0</v>
@@ -2036,27 +2036,39 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="13" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:14" s="13" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A2" s="24" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B2" s="16" t="s">
         <v>40</v>
       </c>
       <c r="C2" s="16" t="s">
+        <v>77</v>
+      </c>
+      <c r="D2" s="16">
+        <v>3</v>
+      </c>
+      <c r="E2" s="21">
+        <v>42672</v>
+      </c>
+      <c r="F2" s="17">
+        <v>0.92361111111111116</v>
+      </c>
+      <c r="G2" s="21"/>
+      <c r="H2" s="49">
+        <f>-(42+(58.6829/60))</f>
+        <v>-42.978048333333334</v>
+      </c>
+      <c r="I2" s="49">
+        <f>-(42+(29.7399/60))</f>
+        <v>-42.495665000000002</v>
+      </c>
+      <c r="J2" s="16">
+        <v>5189</v>
+      </c>
+      <c r="K2" s="16" t="s">
         <v>78</v>
-      </c>
-      <c r="D2" s="16">
-        <v>3</v>
-      </c>
-      <c r="E2" s="21"/>
-      <c r="F2" s="17"/>
-      <c r="G2" s="21"/>
-      <c r="H2" s="16"/>
-      <c r="I2" s="16"/>
-      <c r="J2" s="16"/>
-      <c r="K2" s="16" t="s">
-        <v>79</v>
       </c>
       <c r="L2" s="2"/>
       <c r="M2" s="18" t="e">
@@ -2068,60 +2080,60 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="3" spans="1:14" s="13" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:14" s="13" customFormat="1" x14ac:dyDescent="0.2">
       <c r="E3" s="19"/>
       <c r="F3" s="20"/>
       <c r="G3" s="19"/>
     </row>
-    <row r="4" spans="1:14" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:14" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A4" s="24"/>
     </row>
-    <row r="5" spans="1:14" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:14" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A5" s="24"/>
     </row>
-    <row r="6" spans="1:14" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:14" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A6" s="24"/>
     </row>
-    <row r="7" spans="1:14" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:14" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A7" s="24"/>
     </row>
-    <row r="8" spans="1:14" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:14" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A8" s="24"/>
     </row>
-    <row r="9" spans="1:14" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:14" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A9" s="24"/>
     </row>
-    <row r="10" spans="1:14" s="13" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:14" s="13" customFormat="1" x14ac:dyDescent="0.2">
       <c r="E10" s="19"/>
       <c r="F10" s="20"/>
       <c r="G10" s="19"/>
     </row>
-    <row r="11" spans="1:14" s="13" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:14" s="13" customFormat="1" x14ac:dyDescent="0.2">
       <c r="E11" s="19"/>
       <c r="F11" s="20"/>
       <c r="G11" s="19"/>
     </row>
-    <row r="12" spans="1:14" s="13" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:14" s="13" customFormat="1" x14ac:dyDescent="0.2">
       <c r="E12" s="19"/>
       <c r="F12" s="20"/>
       <c r="G12" s="19"/>
     </row>
-    <row r="13" spans="1:14" s="13" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:14" s="13" customFormat="1" x14ac:dyDescent="0.2">
       <c r="E13" s="19"/>
       <c r="F13" s="20"/>
       <c r="G13" s="19"/>
     </row>
-    <row r="14" spans="1:14" s="13" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:14" s="13" customFormat="1" x14ac:dyDescent="0.2">
       <c r="E14" s="19"/>
       <c r="F14" s="20"/>
       <c r="G14" s="19"/>
     </row>
-    <row r="15" spans="1:14" s="13" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:14" s="13" customFormat="1" x14ac:dyDescent="0.2">
       <c r="E15" s="19"/>
       <c r="F15" s="20"/>
       <c r="G15" s="19"/>
     </row>
-    <row r="16" spans="1:14" s="13" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:14" s="13" customFormat="1" x14ac:dyDescent="0.2">
       <c r="E16" s="19"/>
       <c r="F16" s="20"/>
       <c r="G16" s="19"/>
@@ -2129,11 +2141,6 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -2141,30 +2148,30 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q76"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:E1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A50" workbookViewId="0">
+      <selection activeCell="F86" sqref="F86"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="34.88671875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="20.77734375" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="34.83203125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="20.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.5" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="7.6640625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="20.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="23.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.5" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="27" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="26.6640625" style="1" customWidth="1"/>
-    <col min="9" max="9" width="20.88671875" style="1" customWidth="1"/>
-    <col min="10" max="16384" width="8.88671875" style="1"/>
+    <col min="9" max="9" width="20.83203125" style="1" customWidth="1"/>
+    <col min="10" max="16384" width="8.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="34" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C1" s="10" t="s">
         <v>1</v>
@@ -2173,7 +2180,7 @@
         <v>24</v>
       </c>
       <c r="E1" s="34" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F1" s="10" t="s">
         <v>2</v>
@@ -2188,22 +2195,22 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="3" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="3" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>30</v>
       </c>
       <c r="B3" s="24" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D3" s="1">
         <v>3</v>
       </c>
       <c r="E3" s="24" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F3" s="31">
         <v>3281</v>
@@ -2218,21 +2225,21 @@
         <v>31</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A4" s="25" t="s">
         <v>30</v>
       </c>
       <c r="B4" s="24" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D4" s="1">
         <v>3</v>
       </c>
       <c r="E4" s="24" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F4" s="31">
         <v>3281</v>
@@ -2244,21 +2251,21 @@
         <v>1.6169999999999999E-6</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A5" s="25" t="s">
         <v>30</v>
       </c>
       <c r="B5" s="24" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D5" s="1">
         <v>3</v>
       </c>
       <c r="E5" s="24" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F5" s="31">
         <v>3281</v>
@@ -2270,21 +2277,21 @@
         <v>50</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A6" s="25" t="s">
         <v>30</v>
       </c>
       <c r="B6" s="24" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D6" s="1">
         <v>3</v>
       </c>
       <c r="E6" s="24" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F6" s="31">
         <v>3281</v>
@@ -2296,21 +2303,21 @@
         <v>7.1000000000000004E-3</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A7" s="25" t="s">
         <v>30</v>
       </c>
       <c r="B7" s="24" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D7" s="1">
         <v>3</v>
       </c>
       <c r="E7" s="24" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F7" s="31">
         <v>3281</v>
@@ -2325,21 +2332,21 @@
         <v>24</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A8" s="25" t="s">
         <v>30</v>
       </c>
       <c r="B8" s="24" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D8" s="1">
         <v>3</v>
       </c>
       <c r="E8" s="24" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F8" s="31">
         <v>3281</v>
@@ -2354,21 +2361,21 @@
         <v>25</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A9" s="25" t="s">
         <v>30</v>
       </c>
       <c r="B9" s="24" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D9" s="1">
         <v>3</v>
       </c>
       <c r="E9" s="24" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F9" s="31">
         <v>3281</v>
@@ -2383,21 +2390,21 @@
         <v>25</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A10" s="25" t="s">
         <v>30</v>
       </c>
       <c r="B10" s="24" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D10" s="1">
         <v>3</v>
       </c>
       <c r="E10" s="24" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F10" s="31">
         <v>3281</v>
@@ -2412,26 +2419,26 @@
         <v>25</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="F11" s="26"/>
       <c r="G11" s="26"/>
       <c r="H11" s="26"/>
     </row>
-    <row r="12" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>32</v>
       </c>
       <c r="B12" s="24" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D12" s="1">
         <v>3</v>
       </c>
       <c r="E12" s="24" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F12" s="27">
         <v>1477</v>
@@ -2439,26 +2446,26 @@
       <c r="G12" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="H12" s="47"/>
+      <c r="H12" s="46"/>
       <c r="I12" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A13" s="25" t="s">
         <v>32</v>
       </c>
       <c r="B13" s="24" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D13" s="1">
         <v>3</v>
       </c>
       <c r="E13" s="24" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F13" s="27">
         <v>1477</v>
@@ -2466,28 +2473,28 @@
       <c r="G13" s="26" t="s">
         <v>7</v>
       </c>
-      <c r="H13" s="47"/>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="H13" s="46"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="F14" s="26"/>
       <c r="G14" s="26"/>
       <c r="H14" s="26"/>
     </row>
-    <row r="15" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>33</v>
       </c>
       <c r="B15" s="24" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D15" s="1">
         <v>3</v>
       </c>
       <c r="E15" s="24" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="F15" s="27">
         <v>133</v>
@@ -2495,23 +2502,23 @@
       <c r="G15" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="H15" s="47"/>
-    </row>
-    <row r="16" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="H15" s="46"/>
+    </row>
+    <row r="16" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A16" s="25" t="s">
         <v>33</v>
       </c>
       <c r="B16" s="24" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D16" s="1">
         <v>3</v>
       </c>
       <c r="E16" s="24" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="F16" s="27">
         <v>133</v>
@@ -2519,28 +2526,28 @@
       <c r="G16" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="H16" s="47"/>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="H16" s="46"/>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="F17" s="26"/>
       <c r="G17" s="26"/>
       <c r="H17" s="26"/>
     </row>
-    <row r="18" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>34</v>
       </c>
       <c r="B18" s="24" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D18" s="1">
         <v>3</v>
       </c>
-      <c r="E18" s="46" t="s">
-        <v>88</v>
+      <c r="E18" s="45" t="s">
+        <v>87</v>
       </c>
       <c r="F18" s="27">
         <v>1116</v>
@@ -2548,23 +2555,23 @@
       <c r="G18" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="H18" s="47"/>
-    </row>
-    <row r="19" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="H18" s="46"/>
+    </row>
+    <row r="19" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A19" s="25" t="s">
         <v>34</v>
       </c>
       <c r="B19" s="24" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D19" s="1">
         <v>3</v>
       </c>
-      <c r="E19" s="46" t="s">
-        <v>88</v>
+      <c r="E19" s="45" t="s">
+        <v>87</v>
       </c>
       <c r="F19" s="27">
         <v>1116</v>
@@ -2572,28 +2579,28 @@
       <c r="G19" s="26" t="s">
         <v>7</v>
       </c>
-      <c r="H19" s="47"/>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="H19" s="46"/>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="F20" s="26"/>
       <c r="G20" s="26"/>
       <c r="H20" s="26"/>
     </row>
-    <row r="21" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>35</v>
       </c>
       <c r="B21" s="24" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D21" s="1">
         <v>3</v>
       </c>
       <c r="E21" s="24" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F21" s="27">
         <v>3279</v>
@@ -2608,21 +2615,21 @@
         <v>36</v>
       </c>
     </row>
-    <row r="22" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A22" s="25" t="s">
         <v>35</v>
       </c>
       <c r="B22" s="24" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D22" s="1">
         <v>3</v>
       </c>
       <c r="E22" s="24" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F22" s="27">
         <v>3279</v>
@@ -2634,21 +2641,21 @@
         <v>1.663E-6</v>
       </c>
     </row>
-    <row r="23" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A23" s="25" t="s">
         <v>35</v>
       </c>
       <c r="B23" s="24" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D23" s="1">
         <v>3</v>
       </c>
       <c r="E23" s="24" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F23" s="27">
         <v>3279</v>
@@ -2660,21 +2667,21 @@
         <v>44</v>
       </c>
     </row>
-    <row r="24" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A24" s="25" t="s">
         <v>35</v>
       </c>
       <c r="B24" s="24" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D24" s="1">
         <v>3</v>
       </c>
       <c r="E24" s="24" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F24" s="27">
         <v>3279</v>
@@ -2686,21 +2693,21 @@
         <v>6.8999999999999999E-3</v>
       </c>
     </row>
-    <row r="25" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A25" s="25" t="s">
         <v>35</v>
       </c>
       <c r="B25" s="24" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D25" s="1">
         <v>3</v>
       </c>
       <c r="E25" s="24" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F25" s="27">
         <v>3279</v>
@@ -2715,21 +2722,21 @@
         <v>25</v>
       </c>
     </row>
-    <row r="26" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A26" s="25" t="s">
         <v>35</v>
       </c>
       <c r="B26" s="24" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D26" s="1">
         <v>3</v>
       </c>
       <c r="E26" s="24" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F26" s="27">
         <v>3279</v>
@@ -2744,21 +2751,21 @@
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A27" s="25" t="s">
         <v>35</v>
       </c>
       <c r="B27" s="24" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D27" s="1">
         <v>3</v>
       </c>
       <c r="E27" s="24" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F27" s="27">
         <v>3279</v>
@@ -2773,21 +2780,21 @@
         <v>25</v>
       </c>
     </row>
-    <row r="28" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A28" s="25" t="s">
         <v>35</v>
       </c>
       <c r="B28" s="24" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D28" s="1">
         <v>3</v>
       </c>
       <c r="E28" s="24" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F28" s="27">
         <v>3279</v>
@@ -2802,26 +2809,26 @@
         <v>25</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="F29" s="26"/>
       <c r="G29" s="26"/>
       <c r="H29" s="26"/>
     </row>
-    <row r="30" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
         <v>37</v>
       </c>
       <c r="B30" s="24" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D30" s="1">
         <v>3</v>
       </c>
       <c r="E30" s="24" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F30" s="27">
         <v>1473</v>
@@ -2829,23 +2836,23 @@
       <c r="G30" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="H30" s="47"/>
-    </row>
-    <row r="31" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="H30" s="46"/>
+    </row>
+    <row r="31" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A31" s="25" t="s">
         <v>37</v>
       </c>
       <c r="B31" s="24" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D31" s="1">
         <v>3</v>
       </c>
       <c r="E31" s="24" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F31" s="27">
         <v>1473</v>
@@ -2853,28 +2860,28 @@
       <c r="G31" s="26" t="s">
         <v>7</v>
       </c>
-      <c r="H31" s="47"/>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="H31" s="46"/>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
       <c r="F32" s="26"/>
       <c r="G32" s="26"/>
       <c r="H32" s="26"/>
     </row>
-    <row r="33" spans="1:17" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:17" ht="15" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
         <v>38</v>
       </c>
       <c r="B33" s="24" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D33" s="1">
         <v>3</v>
       </c>
       <c r="E33" s="24" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F33" s="27">
         <v>135</v>
@@ -2882,23 +2889,23 @@
       <c r="G33" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="H33" s="47"/>
-    </row>
-    <row r="34" spans="1:17" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="H33" s="46"/>
+    </row>
+    <row r="34" spans="1:17" ht="15" x14ac:dyDescent="0.2">
       <c r="A34" s="25" t="s">
         <v>38</v>
       </c>
       <c r="B34" s="24" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D34" s="1">
         <v>3</v>
       </c>
       <c r="E34" s="24" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F34" s="27">
         <v>135</v>
@@ -2906,28 +2913,28 @@
       <c r="G34" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="H34" s="47"/>
-    </row>
-    <row r="35" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="H34" s="46"/>
+    </row>
+    <row r="35" spans="1:17" x14ac:dyDescent="0.2">
       <c r="F35" s="26"/>
       <c r="G35" s="26"/>
       <c r="H35" s="26"/>
     </row>
-    <row r="36" spans="1:17" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:17" ht="15" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
         <v>39</v>
       </c>
       <c r="B36" s="24" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D36" s="1">
         <v>3</v>
       </c>
-      <c r="E36" s="46" t="s">
-        <v>92</v>
+      <c r="E36" s="45" t="s">
+        <v>91</v>
       </c>
       <c r="F36" s="27">
         <v>1110</v>
@@ -2935,23 +2942,23 @@
       <c r="G36" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="H36" s="47"/>
-    </row>
-    <row r="37" spans="1:17" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="H36" s="46"/>
+    </row>
+    <row r="37" spans="1:17" ht="15" x14ac:dyDescent="0.2">
       <c r="A37" s="25" t="s">
         <v>39</v>
       </c>
       <c r="B37" s="24" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D37" s="1">
         <v>3</v>
       </c>
-      <c r="E37" s="46" t="s">
-        <v>92</v>
+      <c r="E37" s="45" t="s">
+        <v>91</v>
       </c>
       <c r="F37" s="27">
         <v>1110</v>
@@ -2959,22 +2966,22 @@
       <c r="G37" s="26" t="s">
         <v>7</v>
       </c>
-      <c r="H37" s="47"/>
-    </row>
-    <row r="38" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="H37" s="46"/>
+    </row>
+    <row r="38" spans="1:17" x14ac:dyDescent="0.2">
       <c r="F38" s="26"/>
       <c r="G38" s="26"/>
       <c r="H38" s="26"/>
     </row>
-    <row r="39" spans="1:17" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:17" ht="15" x14ac:dyDescent="0.2">
       <c r="I39" s="24" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="J39" s="1" t="s">
         <v>46</v>
       </c>
       <c r="K39" s="24" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="L39" s="1" t="s">
         <v>41</v>
@@ -2983,20 +2990,20 @@
       <c r="P39" s="26"/>
       <c r="Q39" s="26"/>
     </row>
-    <row r="40" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:17" x14ac:dyDescent="0.2">
       <c r="O40" s="26"/>
       <c r="P40" s="26"/>
       <c r="Q40" s="26"/>
     </row>
-    <row r="41" spans="1:17" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:17" ht="15" x14ac:dyDescent="0.2">
       <c r="I41" s="24" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="J41" s="1" t="s">
         <v>47</v>
       </c>
       <c r="K41" s="24" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="L41" s="1" t="s">
         <v>41</v>
@@ -3006,121 +3013,121 @@
       <c r="P41" s="26"/>
       <c r="Q41" s="26"/>
     </row>
-    <row r="42" spans="1:17" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:17" ht="15" x14ac:dyDescent="0.2">
       <c r="B42" s="24"/>
       <c r="E42" s="24"/>
       <c r="F42" s="26"/>
       <c r="G42" s="26"/>
       <c r="H42" s="26"/>
     </row>
-    <row r="43" spans="1:17" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:17" ht="15" x14ac:dyDescent="0.2">
       <c r="A43" s="22" t="s">
         <v>42</v>
       </c>
       <c r="B43" s="24" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D43" s="1">
         <v>3</v>
       </c>
       <c r="E43" s="24" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F43" s="26" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G43" s="35" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H43" s="36">
         <v>39</v>
       </c>
       <c r="I43" s="37" t="s">
-        <v>54</v>
-      </c>
-      <c r="J43" s="49">
+        <v>53</v>
+      </c>
+      <c r="J43" s="48">
         <v>163</v>
       </c>
       <c r="L43" s="26"/>
       <c r="M43" s="26"/>
     </row>
-    <row r="44" spans="1:17" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:17" ht="15" x14ac:dyDescent="0.2">
       <c r="A44" s="42" t="s">
         <v>42</v>
       </c>
       <c r="B44" s="24" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D44" s="1">
         <v>3</v>
       </c>
       <c r="E44" s="24" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F44" s="42" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G44" s="35" t="s">
         <v>6</v>
       </c>
-      <c r="H44" s="48"/>
+      <c r="H44" s="47"/>
       <c r="I44" s="37"/>
       <c r="J44" s="37"/>
       <c r="L44" s="26"/>
       <c r="M44" s="41"/>
     </row>
-    <row r="45" spans="1:17" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:17" ht="15" x14ac:dyDescent="0.2">
       <c r="A45" s="42" t="s">
         <v>42</v>
       </c>
       <c r="B45" s="24" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D45" s="1">
         <v>3</v>
       </c>
       <c r="E45" s="24" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F45" s="42" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G45" s="35" t="s">
         <v>7</v>
       </c>
-      <c r="H45" s="48"/>
+      <c r="H45" s="47"/>
       <c r="I45" s="37"/>
       <c r="J45" s="37"/>
       <c r="L45" s="26"/>
       <c r="M45" s="41"/>
     </row>
-    <row r="46" spans="1:17" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:17" ht="15" x14ac:dyDescent="0.2">
       <c r="A46" s="42" t="s">
         <v>42</v>
       </c>
       <c r="B46" s="24" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D46" s="1">
         <v>3</v>
       </c>
       <c r="E46" s="24" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F46" s="42" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G46" s="35" t="s">
         <v>5</v>
@@ -3133,27 +3140,27 @@
       <c r="L46" s="26"/>
       <c r="M46" s="41"/>
     </row>
-    <row r="47" spans="1:17" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:17" ht="15" x14ac:dyDescent="0.2">
       <c r="A47" s="42" t="s">
         <v>42</v>
       </c>
       <c r="B47" s="24" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D47" s="1">
         <v>3</v>
       </c>
       <c r="E47" s="24" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F47" s="42" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G47" s="38" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="H47" s="43">
         <v>7.4214999999999996E-7</v>
@@ -3162,27 +3169,27 @@
       <c r="L47" s="26"/>
       <c r="M47" s="41"/>
     </row>
-    <row r="48" spans="1:17" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:17" ht="15" x14ac:dyDescent="0.2">
       <c r="A48" s="42" t="s">
         <v>42</v>
       </c>
       <c r="B48" s="24" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D48" s="1">
         <v>3</v>
       </c>
       <c r="E48" s="24" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F48" s="42" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G48" s="39" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H48" s="44">
         <v>-1.27498E-4</v>
@@ -3191,27 +3198,27 @@
       <c r="L48" s="26"/>
       <c r="M48" s="41"/>
     </row>
-    <row r="49" spans="1:13" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:13" ht="15" x14ac:dyDescent="0.2">
       <c r="A49" s="42" t="s">
         <v>42</v>
       </c>
       <c r="B49" s="24" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D49" s="1">
         <v>3</v>
       </c>
       <c r="E49" s="24" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F49" s="42" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G49" s="39" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="H49" s="44">
         <v>3.1112959999999998E-4</v>
@@ -3220,27 +3227,27 @@
       <c r="L49" s="26"/>
       <c r="M49" s="41"/>
     </row>
-    <row r="50" spans="1:13" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:13" ht="15" x14ac:dyDescent="0.2">
       <c r="A50" s="42" t="s">
         <v>42</v>
       </c>
       <c r="B50" s="24" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D50" s="1">
         <v>3</v>
       </c>
       <c r="E50" s="24" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F50" s="42" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G50" s="39" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="H50" s="44">
         <v>-4.7930340000000002E-6</v>
@@ -3249,27 +3256,27 @@
       <c r="L50" s="26"/>
       <c r="M50" s="41"/>
     </row>
-    <row r="51" spans="1:13" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:13" ht="15" x14ac:dyDescent="0.2">
       <c r="A51" s="42" t="s">
         <v>42</v>
       </c>
       <c r="B51" s="24" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D51" s="1">
         <v>3</v>
       </c>
       <c r="E51" s="24" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F51" s="42" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G51" s="39" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H51" s="44">
         <v>2.102939E-7</v>
@@ -3278,27 +3285,27 @@
       <c r="L51" s="26"/>
       <c r="M51" s="41"/>
     </row>
-    <row r="52" spans="1:13" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:13" ht="15" x14ac:dyDescent="0.2">
       <c r="A52" s="42" t="s">
         <v>42</v>
       </c>
       <c r="B52" s="24" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D52" s="1">
         <v>3</v>
       </c>
       <c r="E52" s="24" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F52" s="42" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G52" s="39" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H52" s="43">
         <v>-70.319659999999999</v>
@@ -3307,27 +3314,27 @@
       <c r="L52" s="26"/>
       <c r="M52" s="41"/>
     </row>
-    <row r="53" spans="1:13" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:13" ht="15" x14ac:dyDescent="0.2">
       <c r="A53" s="42" t="s">
         <v>42</v>
       </c>
       <c r="B53" s="24" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D53" s="1">
         <v>3</v>
       </c>
       <c r="E53" s="24" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F53" s="42" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G53" s="39" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="H53" s="43">
         <v>5.0888830000000003E-2</v>
@@ -3336,27 +3343,27 @@
       <c r="L53" s="26"/>
       <c r="M53" s="41"/>
     </row>
-    <row r="54" spans="1:13" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:13" ht="15" x14ac:dyDescent="0.2">
       <c r="A54" s="42" t="s">
         <v>42</v>
       </c>
       <c r="B54" s="24" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D54" s="1">
         <v>3</v>
       </c>
       <c r="E54" s="24" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F54" s="42" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G54" s="39" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H54" s="43">
         <v>-4.9473889999999998E-7</v>
@@ -3365,27 +3372,27 @@
       <c r="L54" s="26"/>
       <c r="M54" s="41"/>
     </row>
-    <row r="55" spans="1:13" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:13" ht="15" x14ac:dyDescent="0.2">
       <c r="A55" s="42" t="s">
         <v>42</v>
       </c>
       <c r="B55" s="24" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D55" s="1">
         <v>3</v>
       </c>
       <c r="E55" s="24" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F55" s="42" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G55" s="39" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H55" s="43">
         <v>524920.1</v>
@@ -3394,27 +3401,27 @@
       <c r="L55" s="26"/>
       <c r="M55" s="41"/>
     </row>
-    <row r="56" spans="1:13" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:13" ht="15" x14ac:dyDescent="0.2">
       <c r="A56" s="42" t="s">
         <v>42</v>
       </c>
       <c r="B56" s="24" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D56" s="1">
         <v>3</v>
       </c>
       <c r="E56" s="24" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F56" s="42" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G56" s="39" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="H56" s="43">
         <v>3.2037740000000001</v>
@@ -3423,27 +3430,27 @@
       <c r="L56" s="26"/>
       <c r="M56" s="41"/>
     </row>
-    <row r="57" spans="1:13" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:13" ht="15" x14ac:dyDescent="0.2">
       <c r="A57" s="42" t="s">
         <v>42</v>
       </c>
       <c r="B57" s="24" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D57" s="1">
         <v>3</v>
       </c>
       <c r="E57" s="24" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F57" s="42" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G57" s="39" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="H57" s="43">
         <v>1.9005500000000002E-2</v>
@@ -3452,27 +3459,27 @@
       <c r="L57" s="26"/>
       <c r="M57" s="41"/>
     </row>
-    <row r="58" spans="1:13" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:13" ht="15" x14ac:dyDescent="0.2">
       <c r="A58" s="42" t="s">
         <v>42</v>
       </c>
       <c r="B58" s="24" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D58" s="1">
         <v>3</v>
       </c>
       <c r="E58" s="24" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F58" s="42" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G58" s="39" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="H58" s="43">
         <v>25.09337</v>
@@ -3481,27 +3488,27 @@
       <c r="L58" s="26"/>
       <c r="M58" s="41"/>
     </row>
-    <row r="59" spans="1:13" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:13" ht="15" x14ac:dyDescent="0.2">
       <c r="A59" s="42" t="s">
         <v>42</v>
       </c>
       <c r="B59" s="24" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D59" s="1">
         <v>3</v>
       </c>
       <c r="E59" s="24" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F59" s="42" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G59" s="39" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="H59" s="43">
         <v>3.6749999999999999E-3</v>
@@ -3510,27 +3517,27 @@
       <c r="L59" s="26"/>
       <c r="M59" s="41"/>
     </row>
-    <row r="60" spans="1:13" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:13" ht="15" x14ac:dyDescent="0.2">
       <c r="A60" s="42" t="s">
         <v>42</v>
       </c>
       <c r="B60" s="24" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D60" s="1">
         <v>3</v>
       </c>
       <c r="E60" s="24" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F60" s="42" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G60" s="39" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="H60" s="43">
         <v>0</v>
@@ -3539,27 +3546,27 @@
       <c r="L60" s="26"/>
       <c r="M60" s="41"/>
     </row>
-    <row r="61" spans="1:13" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:13" ht="15" x14ac:dyDescent="0.2">
       <c r="A61" s="42" t="s">
         <v>42</v>
       </c>
       <c r="B61" s="24" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D61" s="1">
         <v>3</v>
       </c>
       <c r="E61" s="24" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F61" s="42" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G61" s="39" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="H61" s="44">
         <v>0.20313410000000001</v>
@@ -3568,27 +3575,27 @@
       <c r="L61" s="26"/>
       <c r="M61" s="41"/>
     </row>
-    <row r="62" spans="1:13" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:13" ht="15" x14ac:dyDescent="0.2">
       <c r="A62" s="42" t="s">
         <v>42</v>
       </c>
       <c r="B62" s="24" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D62" s="1">
         <v>3</v>
       </c>
       <c r="E62" s="24" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F62" s="42" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G62" s="39" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="H62" s="44">
         <v>4.4707310000000004E-3</v>
@@ -3597,27 +3604,27 @@
       <c r="L62" s="26"/>
       <c r="M62" s="41"/>
     </row>
-    <row r="63" spans="1:13" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:13" ht="15" x14ac:dyDescent="0.2">
       <c r="A63" s="42" t="s">
         <v>42</v>
       </c>
       <c r="B63" s="24" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D63" s="1">
         <v>3</v>
       </c>
       <c r="E63" s="24" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F63" s="42" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G63" s="39" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H63" s="44">
         <v>-1.5900840000000002E-11</v>
@@ -3626,27 +3633,27 @@
       <c r="L63" s="26"/>
       <c r="M63" s="41"/>
     </row>
-    <row r="64" spans="1:13" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:13" ht="15" x14ac:dyDescent="0.2">
       <c r="A64" s="42" t="s">
         <v>42</v>
       </c>
       <c r="B64" s="24" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D64" s="1">
         <v>3</v>
       </c>
       <c r="E64" s="24" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F64" s="42" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G64" s="39" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H64" s="43">
         <v>-0.99648789999999998</v>
@@ -3655,27 +3662,27 @@
       <c r="L64" s="26"/>
       <c r="M64" s="41"/>
     </row>
-    <row r="65" spans="1:13" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:13" ht="15" x14ac:dyDescent="0.2">
       <c r="A65" s="42" t="s">
         <v>42</v>
       </c>
       <c r="B65" s="24" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D65" s="1">
         <v>3</v>
       </c>
       <c r="E65" s="24" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F65" s="42" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G65" s="39" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="H65" s="43">
         <v>0.1641842</v>
@@ -3684,27 +3691,27 @@
       <c r="L65" s="26"/>
       <c r="M65" s="41"/>
     </row>
-    <row r="66" spans="1:13" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:13" ht="15" x14ac:dyDescent="0.2">
       <c r="A66" s="42" t="s">
         <v>42</v>
       </c>
       <c r="B66" s="24" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D66" s="1">
         <v>3</v>
       </c>
       <c r="E66" s="24" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F66" s="42" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G66" s="39" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="H66" s="43">
         <v>-5.3294699999999998E-4</v>
@@ -3713,27 +3720,27 @@
       <c r="L66" s="26"/>
       <c r="M66" s="41"/>
     </row>
-    <row r="67" spans="1:13" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:13" ht="15" x14ac:dyDescent="0.2">
       <c r="A67" s="42" t="s">
         <v>42</v>
       </c>
       <c r="B67" s="24" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D67" s="1">
         <v>3</v>
       </c>
       <c r="E67" s="24" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F67" s="42" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G67" s="39" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="H67" s="43">
         <v>6.609059E-5</v>
@@ -3742,27 +3749,27 @@
       <c r="L67" s="26"/>
       <c r="M67" s="41"/>
     </row>
-    <row r="68" spans="1:13" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:13" ht="15" x14ac:dyDescent="0.2">
       <c r="A68" s="42" t="s">
         <v>42</v>
       </c>
       <c r="B68" s="24" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D68" s="1">
         <v>3</v>
       </c>
       <c r="E68" s="24" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F68" s="42" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G68" s="39" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="H68" s="43">
         <v>-9.5700000000000003E-8</v>
@@ -3771,27 +3778,27 @@
       <c r="L68" s="26"/>
       <c r="M68" s="41"/>
     </row>
-    <row r="69" spans="1:13" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:13" ht="15" x14ac:dyDescent="0.2">
       <c r="A69" s="42" t="s">
         <v>42</v>
       </c>
       <c r="B69" s="24" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D69" s="1">
         <v>3</v>
       </c>
       <c r="E69" s="24" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F69" s="42" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G69" s="39" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="H69" s="43">
         <v>3.2499999999999998E-6</v>
@@ -3800,91 +3807,91 @@
       <c r="L69" s="26"/>
       <c r="M69" s="41"/>
     </row>
-    <row r="70" spans="1:13" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:13" ht="15" x14ac:dyDescent="0.2">
       <c r="B70" s="24"/>
       <c r="E70" s="24"/>
       <c r="F70" s="26"/>
       <c r="G70" s="26"/>
       <c r="H70" s="26"/>
     </row>
-    <row r="71" spans="1:13" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:13" ht="15" x14ac:dyDescent="0.2">
       <c r="A71" s="22" t="s">
         <v>45</v>
       </c>
       <c r="B71" s="24" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D71" s="1">
         <v>3</v>
       </c>
       <c r="E71" s="24"/>
-      <c r="F71" s="45" t="s">
-        <v>48</v>
+      <c r="F71" s="29">
+        <v>13988</v>
       </c>
       <c r="G71" s="29"/>
       <c r="H71" s="29"/>
       <c r="I71" s="23"/>
     </row>
-    <row r="72" spans="1:13" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:13" ht="15" x14ac:dyDescent="0.2">
       <c r="A72" s="22" t="s">
         <v>43</v>
       </c>
       <c r="B72" s="24" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D72" s="1">
         <v>3</v>
       </c>
       <c r="E72" s="24" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F72" s="28" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="G72" s="26"/>
       <c r="H72" s="26"/>
       <c r="I72" s="23"/>
     </row>
-    <row r="73" spans="1:13" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:13" ht="15" x14ac:dyDescent="0.2">
       <c r="A73" s="22" t="s">
         <v>44</v>
       </c>
       <c r="B73" s="24" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D73" s="1">
         <v>3</v>
       </c>
       <c r="E73" s="24" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F73" s="28" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="G73" s="26"/>
       <c r="H73" s="26"/>
       <c r="I73" s="23"/>
     </row>
-    <row r="74" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:13" x14ac:dyDescent="0.2">
       <c r="F74" s="26"/>
       <c r="G74" s="26"/>
       <c r="H74" s="26"/>
     </row>
-    <row r="75" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:13" x14ac:dyDescent="0.2">
       <c r="F75" s="26"/>
       <c r="G75" s="26"/>
       <c r="H75" s="26"/>
     </row>
-    <row r="76" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:13" x14ac:dyDescent="0.2">
       <c r="F76" s="26"/>
       <c r="G76" s="26"/>
       <c r="H76" s="26"/>
@@ -3892,10 +3899,5 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
</xml_diff>